<commit_message>
Updated 125I Radioactive Disposal Log & Printout
</commit_message>
<xml_diff>
--- a/Python_Scripts/I125_Binding/data_files/125I-Binding_Printout_Template.xlsx
+++ b/Python_Scripts/I125_Binding/data_files/125I-Binding_Printout_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kealbert\Documents\PDSP\Python_Scripts\I125_Binding\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E991DCD-5AFD-417F-A247-638AEECA808B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919829F5-D184-4C4C-AA92-4BA076E781BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="20490" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,13 +88,13 @@
     <t># of Pellets</t>
   </si>
   <si>
-    <t>Ligand (µCi)</t>
-  </si>
-  <si>
     <t>125I Binding Worksheet</t>
   </si>
   <si>
     <t>125I-Ligand</t>
+  </si>
+  <si>
+    <t>Ligand (mCi)</t>
   </si>
 </sst>
 </file>
@@ -364,9 +364,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -391,6 +388,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1153,7 +1153,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,21 +1172,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="28"/>
+      <c r="A1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1199,24 +1199,24 @@
       <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="32"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="31"/>
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1228,15 +1228,15 @@
         <v>16</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="37"/>
+      <c r="I3" s="36"/>
       <c r="J3" s="17" t="s">
         <v>9</v>
       </c>
@@ -1251,7 +1251,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="5"/>
@@ -1260,159 +1260,159 @@
       <c r="E4" s="6"/>
       <c r="F4" s="23"/>
       <c r="G4" s="19"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
       <c r="J4" s="13"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="5"/>
       <c r="C5" s="11"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="23"/>
       <c r="G5" s="19"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="13"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="5"/>
       <c r="C6" s="11"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="23"/>
       <c r="G6" s="19"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
       <c r="J6" s="13"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="5"/>
       <c r="C7" s="11"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="23"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="13"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="5"/>
       <c r="C8" s="11"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="23"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="13"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="5"/>
       <c r="C9" s="11"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="23"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="13"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="5"/>
       <c r="C10" s="11"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="23"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
       <c r="J10" s="13"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="5"/>
       <c r="C11" s="11"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="23"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="13"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="3"/>
       <c r="C12" s="12"/>
       <c r="D12" s="7"/>
       <c r="E12" s="6"/>
       <c r="F12" s="24"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="13"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="25" t="s">
+      <c r="B13" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="38" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="13"/>
@@ -1421,15 +1421,15 @@
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="13"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -1695,6 +1695,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:M2"/>
@@ -1709,15 +1718,6 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
   </mergeCells>
   <conditionalFormatting sqref="A15:I15">
     <cfRule type="expression" dxfId="43" priority="10">

</xml_diff>